<commit_message>
the about the work.xlsx which is modified...
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitlearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F42353-3182-4FED-BCE3-22BCAB9256E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A483A248-93C7-42C2-B612-C533DCCA2F19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>This is microsoft word sheet</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Khan</t>
+  </si>
+  <si>
+    <t>Sailen</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +407,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>